<commit_message>
PROVA - altri commenti
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/Problemi_veicoli.xlsx
+++ b/PS-VRP/Dati_output/Problemi_veicoli.xlsx
@@ -26,12 +26,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,8 +52,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +420,83 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>nome</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>peso</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>zone</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>partenza</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>40279 (interno)</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>40176 (interno)</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>